<commit_message>
Add unit tests for probabilities and first part in grid
</commit_message>
<xml_diff>
--- a/lab_3/output.xlsx
+++ b/lab_3/output.xlsx
@@ -35321,8 +35321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>